<commit_message>
change server dir names(for deploy and tools) add bus plugin(unfinished, for deploy)
Former-commit-id: f53e9e72aad4d393b98bc573389542636d60f991 [formerly b0bcf7ceab4dffbaeda9c75bfe8bf66e00c0d1b1] [formerly b71c26930a006a6a06a0ef2bb34b46578ae3966b [formerly 663089358b810582db85663b74ddef17efb01028]]
Former-commit-id: 4f9b2e1923d54d6b754db4d99309ad2a6a88f554 [formerly 2ad2a89c4d639c12cb30952105dca3b92915a9a4]
Former-commit-id: 4f679f869c01e8aa8defff0fbe0fbbbe3c66cdda
</commit_message>
<xml_diff>
--- a/Bin/Server/DataConfig/Excel/Server.xlsx
+++ b/Bin/Server/DataConfig/Excel/Server.xlsx
@@ -1,33 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\ArkGameFrame\Bin\Server\DataConfig\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="27765" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
   <si>
     <t>Id</t>
   </si>
@@ -98,44 +85,50 @@
     <t>服务器类型</t>
   </si>
   <si>
+    <t>MasterServer_1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
+  </si>
+  <si>
+    <t>WorldServer_1</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
     <t>GameServer_1</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>127.0.0.1</t>
-  </si>
-  <si>
-    <t>WorldServer_1</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>51</t>
+  </si>
+  <si>
+    <t>LoginServer_1</t>
+  </si>
+  <si>
+    <t>52</t>
   </si>
   <si>
     <t>ProxyServer_1</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>MasterServer_1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>LoginServer_1</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>53</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -155,12 +148,158 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +318,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -304,9 +629,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -360,17 +927,61 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -699,20 +1310,21 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="28.125" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -724,7 +1336,7 @@
     <col min="8" max="8" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="1" s="1" customFormat="1" ht="27" spans="1:8">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -750,7 +1362,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" s="2" customFormat="1" spans="1:8">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -776,7 +1388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" s="2" customFormat="1" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
@@ -802,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" s="2" customFormat="1" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -828,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" s="2" customFormat="1" spans="1:8">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
@@ -854,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" s="2" customFormat="1" spans="1:8">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -880,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" s="3" customFormat="1" spans="1:8">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -906,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="8" s="4" customFormat="1" ht="41.25" spans="1:8">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -932,14 +1544,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9">
@@ -952,13 +1564,13 @@
         <v>25</v>
       </c>
       <c r="G9">
-        <v>16001</v>
+        <v>13001</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
@@ -984,14 +1596,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8">
       <c r="A11" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D11">
@@ -1004,20 +1616,20 @@
         <v>25</v>
       </c>
       <c r="G11">
-        <v>15001</v>
+        <v>16001</v>
       </c>
       <c r="H11" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D12">
@@ -1029,21 +1641,21 @@
       <c r="F12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G12">
-        <v>13001</v>
-      </c>
-      <c r="H12" s="13" t="s">
+      <c r="G12" s="15">
+        <v>14001</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" t="s">
         <v>32</v>
       </c>
       <c r="D13">
@@ -1055,22 +1667,21 @@
       <c r="F13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="15">
-        <v>14001</v>
-      </c>
-      <c r="H13" s="14" t="s">
+      <c r="G13">
+        <v>15001</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:J7 F8 F2:F6 F14:F1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:J7 F8 F2:F6 F14:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
change BusPlugin configuration; Add AFCProcModule in BusPlugin; Change process enum and name;
Former-commit-id: dcf7267a32d156dd9b162e0120b27b87058095c5 [formerly abf10665891460b4b906586ca708b85326e6e1e7] [formerly cac4021f241b990da680aff4e1e9d6d80722b1cb [formerly a2327a03d5714261811fbcc525105c1cf25895fb]]
Former-commit-id: ba93aa35bad2584b544053844270371efa900c59 [formerly b3e8ab9782df8ba3b6b410ca5b80d6dfe0ed09fe]
Former-commit-id: aefc932acc772f5aa5e29d246136dbc795bf743e
</commit_message>
<xml_diff>
--- a/Bin/Server/DataConfig/Excel/Server.xlsx
+++ b/Bin/Server/DataConfig/Excel/Server.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARK\Bin\Server\DataConfig\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="13650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27765" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Id</t>
   </si>
@@ -97,38 +102,58 @@
     <t>WorldServer_1</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>GameServer_1</t>
   </si>
   <si>
-    <t>51</t>
-  </si>
-  <si>
     <t>LoginServer_1</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
     <t>ProxyServer_1</t>
   </si>
   <si>
-    <t>53</t>
+    <t>100</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>01</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <r>
+      <t>103</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t/>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -148,158 +173,19 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,194 +204,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -629,255 +329,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -926,62 +384,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1310,21 +727,20 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="28.125" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
@@ -1336,7 +752,7 @@
     <col min="8" max="8" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="27" spans="1:8">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1362,7 +778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:8">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -1388,7 +804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:8">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
@@ -1414,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:8">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -1440,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:8">
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
@@ -1466,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:8">
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1492,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:8">
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
@@ -1518,7 +934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" s="4" customFormat="1" ht="41.25" spans="1:8">
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -1544,7 +960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -1570,12 +986,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -1593,18 +1009,18 @@
         <v>17001</v>
       </c>
       <c r="H10" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>29</v>
+      <c r="B11" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>5000</v>
@@ -1618,19 +1034,19 @@
       <c r="G11">
         <v>16001</v>
       </c>
-      <c r="H11" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>5000</v>
@@ -1644,19 +1060,19 @@
       <c r="G12" s="15">
         <v>14001</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="H12" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13">
         <v>5000</v>
@@ -1670,19 +1086,20 @@
       <c r="G13">
         <v>15001</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="16" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:J7 F8 F2:F6 F14:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>